<commit_message>
made some changes in the data validation and filtering
</commit_message>
<xml_diff>
--- a/Templates/Heat_and_Steam.xlsx
+++ b/Templates/Heat_and_Steam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Data Life\internship backend developer\batch input\Batch-input-Page\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\LevelUPESG\Batch-input-Page\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5768AD2-2569-402F-83C0-F70BDF663ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E1024C-5B14-40C6-B24C-330CEEA03FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat and Steam" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -551,7 +551,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -630,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -660,17 +660,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
     <dxf>
       <font>
         <color theme="2" tint="-0.499984740745262"/>
@@ -693,28 +690,63 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4472C4"/>
-          <bgColor rgb="FF4472C4"/>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -769,37 +801,42 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color rgb="FF8EA9DB"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF8EA9DB"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF8EA9DB"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <font>
-        <color theme="1" tint="0.499984740745262"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -815,20 +852,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}" name="Table1" displayName="Table1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}" name="Table1" displayName="Table1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="A1:K1048576" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9DF3A374-131F-43B6-9C39-C775FD7A98A5}" name="Asset Name" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{ED5AAC26-EB23-4F53-A995-E89DC3FF9EE8}" name="Asset Type" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{979BFCB7-7060-4B72-BBD7-A782ABC94E77}" name="Reporting Year" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A2C51EF0-723B-4C20-A235-2C621CE89D87}" name="Value Type" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{C6DC634F-BE90-405E-BD48-D59C49E831A6}" name="Consumption (kWh)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{A27BE819-CED3-47A8-9E36-A58D5807A455}" name="Typology" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{1748C08D-AF86-4EE8-9C7E-87CEAE19F1AD}" name="Total Spend" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{533AE4F7-857C-45AA-A9BD-1EC5B97FE058}" name="Currency " dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{FCA8F460-9AE1-4AB7-8E80-35EB816AB9DB}" name="Actual/Estimated" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{DD668173-3319-4CAD-9D50-7A3BF0641F5E}" name="Assumption basis" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{9413C750-1B04-417C-ACB9-427403AD8C21}" name="Evidence" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{9DF3A374-131F-43B6-9C39-C775FD7A98A5}" name="Asset Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{ED5AAC26-EB23-4F53-A995-E89DC3FF9EE8}" name="Asset Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{979BFCB7-7060-4B72-BBD7-A782ABC94E77}" name="Reporting Year" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A2C51EF0-723B-4C20-A235-2C621CE89D87}" name="Value Type" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{C6DC634F-BE90-405E-BD48-D59C49E831A6}" name="Consumption (kWh)" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A27BE819-CED3-47A8-9E36-A58D5807A455}" name="Typology" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{1748C08D-AF86-4EE8-9C7E-87CEAE19F1AD}" name="Total Spend" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{533AE4F7-857C-45AA-A9BD-1EC5B97FE058}" name="Currency " dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{FCA8F460-9AE1-4AB7-8E80-35EB816AB9DB}" name="Actual/Estimated" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{DD668173-3319-4CAD-9D50-7A3BF0641F5E}" name="Assumption basis" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{9413C750-1B04-417C-ACB9-427403AD8C21}" name="Evidence" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1153,27 +1190,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D775E0E9-E192-457C-A3B8-47F95293021D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="1"/>
+    <col min="1" max="1" width="46.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1227,10 +1264,10 @@
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
@@ -1241,27 +1278,17 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="expression" dxfId="17" priority="3">
-      <formula>$D:$D="Total Spend"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="expression" dxfId="16" priority="5">
-      <formula>$D:$D ="Consumption"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="E2:F1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$D2 &lt;&gt; "Consumption "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G2:H1048575">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$D2 &lt;&gt; "Total Spend"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{F8764847-9C39-4CD8-A2DB-642B0361E72F}">
       <formula1>"estimated, actual"</formula1>
     </dataValidation>
@@ -1271,13 +1298,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{E8E9EA8B-F502-456B-8568-B3A4675F91E0}">
       <formula1>"Consumption ,Total Spend"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1048576" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 C1:C2" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
       <formula1>2020</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{06635ADA-7664-4747-91AB-2EB240994011}">
       <formula1>"Onsite heat and steam,District heat and steam"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{C8B4DF01-70D4-4C4C-B6B9-547A38C4AF08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3:B1048576" xr:uid="{C8B4DF01-70D4-4C4C-B6B9-547A38C4AF08}">
       <formula1>"Heat and Steam"</formula1>
     </dataValidation>
     <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{9DEC22D6-A9B9-4942-B6B3-A759EF71BB17}">
@@ -1285,6 +1312,9 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{A931B69C-F657-4E55-A7D7-D60577855578}">
       <formula1>$D2 = "Total Spend"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{45605CBE-FD23-4A0E-A03A-B5C065317735}">
+      <formula1>2020</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1314,1932 +1344,1932 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.125" style="5"/>
+    <col min="3" max="3" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>86</v>
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>108</v>
       </c>
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>112</v>
       </c>
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
         <v>113</v>
       </c>
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>114</v>
       </c>
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>115</v>
       </c>
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>116</v>
       </c>
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>117</v>
       </c>
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>118</v>
       </c>
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>119</v>
       </c>
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>120</v>
       </c>
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>121</v>
       </c>
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>122</v>
       </c>
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>124</v>
       </c>
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>125</v>
       </c>
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>126</v>
       </c>
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>128</v>
       </c>
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
         <v>130</v>
       </c>
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
         <v>131</v>
       </c>
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
         <v>133</v>
       </c>
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>134</v>
       </c>
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>135</v>
       </c>
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
         <v>136</v>
       </c>
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
         <v>137</v>
       </c>
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
         <v>138</v>
       </c>
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>139</v>
       </c>
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="7" t="s">
         <v>141</v>
       </c>
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
         <v>143</v>
       </c>
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>145</v>
       </c>
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
         <v>147</v>
       </c>
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
         <v>148</v>
       </c>
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>149</v>
       </c>
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>152</v>
       </c>
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>153</v>
       </c>
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
         <v>154</v>
       </c>
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>155</v>
       </c>
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="8" t="s">
         <v>156</v>
       </c>
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C200" s="4"/>
     </row>
-    <row r="201" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C201" s="4"/>
     </row>
-    <row r="202" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C202" s="4"/>
     </row>
-    <row r="203" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C203" s="4"/>
     </row>
-    <row r="204" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C204" s="4"/>
     </row>
-    <row r="205" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C205" s="4"/>
     </row>
-    <row r="206" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C206" s="4"/>
     </row>
-    <row r="207" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C207" s="4"/>
     </row>
-    <row r="208" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C224" s="4"/>
     </row>
-    <row r="225" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C225" s="4"/>
     </row>
-    <row r="226" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C226" s="4"/>
     </row>
-    <row r="227" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C227" s="4"/>
     </row>
-    <row r="228" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C228" s="4"/>
     </row>
-    <row r="229" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C229" s="4"/>
     </row>
-    <row r="230" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C230" s="4"/>
     </row>
-    <row r="231" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C231" s="4"/>
     </row>
-    <row r="232" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C232" s="4"/>
     </row>
-    <row r="233" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C233" s="4"/>
     </row>
-    <row r="234" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C234" s="4"/>
     </row>
-    <row r="235" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C235" s="4"/>
     </row>
-    <row r="236" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C238" s="4"/>
     </row>
-    <row r="239" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C239" s="4"/>
     </row>
-    <row r="240" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C240" s="4"/>
     </row>
-    <row r="241" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" s="4"/>
     </row>
-    <row r="242" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" s="4"/>
     </row>
-    <row r="243" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" s="4"/>
     </row>
-    <row r="244" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C244" s="4"/>
     </row>
-    <row r="245" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C245" s="4"/>
     </row>
-    <row r="246" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C246" s="4"/>
     </row>
-    <row r="247" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C247" s="4"/>
     </row>
-    <row r="248" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C248" s="4"/>
     </row>
-    <row r="249" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C249" s="4"/>
     </row>
-    <row r="250" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C250" s="3"/>
     </row>
-    <row r="251" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C251" s="3"/>
     </row>
-    <row r="252" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C252" s="3"/>
     </row>
-    <row r="253" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C253" s="3"/>
     </row>
-    <row r="254" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C254" s="3"/>
     </row>
-    <row r="255" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C255" s="3"/>
     </row>
-    <row r="256" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C256" s="3"/>
     </row>
-    <row r="257" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C257" s="3"/>
     </row>
-    <row r="258" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C258" s="3"/>
     </row>
-    <row r="259" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C259" s="3"/>
     </row>
-    <row r="260" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C260" s="3"/>
     </row>
-    <row r="261" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C261" s="3"/>
     </row>
-    <row r="262" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C262" s="3"/>
     </row>
-    <row r="263" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C263" s="3"/>
     </row>
-    <row r="264" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C264" s="3"/>
     </row>
-    <row r="265" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C265" s="3"/>
     </row>
-    <row r="266" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C266" s="3"/>
     </row>
-    <row r="267" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C267" s="3"/>
     </row>
-    <row r="268" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C268" s="3"/>
     </row>
-    <row r="269" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C269" s="3"/>
     </row>
-    <row r="270" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C270" s="3"/>
     </row>
-    <row r="271" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C271" s="3"/>
     </row>
-    <row r="272" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C272" s="3"/>
     </row>
-    <row r="273" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C273" s="3"/>
     </row>
-    <row r="274" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C274" s="3"/>
     </row>
-    <row r="275" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C275" s="3"/>
     </row>
-    <row r="276" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C276" s="3"/>
     </row>
-    <row r="277" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C277" s="3"/>
     </row>
-    <row r="278" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C278" s="3"/>
     </row>
-    <row r="279" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C279" s="3"/>
     </row>
-    <row r="280" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C280" s="3"/>
     </row>
-    <row r="281" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C281" s="3"/>
     </row>
-    <row r="282" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C282" s="3"/>
     </row>
-    <row r="283" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C283" s="3"/>
     </row>
-    <row r="284" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C284" s="3"/>
     </row>
-    <row r="285" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C285" s="3"/>
     </row>
-    <row r="286" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C286" s="3"/>
     </row>
-    <row r="287" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C287" s="3"/>
     </row>
-    <row r="288" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C288" s="3"/>
     </row>
-    <row r="289" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C289" s="3"/>
     </row>
-    <row r="290" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C290" s="3"/>
     </row>
-    <row r="291" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C291" s="3"/>
     </row>
-    <row r="292" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C292" s="3"/>
     </row>
-    <row r="293" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C293" s="3"/>
     </row>
-    <row r="294" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C294" s="3"/>
     </row>
-    <row r="295" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C296" s="3"/>
     </row>
-    <row r="297" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C297" s="4"/>
     </row>
-    <row r="298" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C298" s="3"/>
     </row>
-    <row r="299" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C299" s="4"/>
     </row>
-    <row r="300" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C300" s="3"/>
     </row>
-    <row r="301" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C301" s="4"/>
     </row>
-    <row r="302" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C302" s="3"/>
     </row>
-    <row r="303" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C303" s="4"/>
     </row>
-    <row r="304" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C304" s="3"/>
     </row>
-    <row r="305" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C305" s="3"/>
     </row>
-    <row r="306" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C306" s="3"/>
     </row>
-    <row r="307" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C307" s="3"/>
     </row>
-    <row r="308" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C308" s="3"/>
     </row>
-    <row r="309" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C309" s="3"/>
     </row>
-    <row r="310" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C310" s="3"/>
     </row>
-    <row r="311" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C311" s="4"/>
     </row>
-    <row r="312" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C312" s="4"/>
     </row>
-    <row r="313" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C313" s="4"/>
     </row>
-    <row r="314" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C314" s="4"/>
     </row>
-    <row r="315" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C315" s="4"/>
     </row>
-    <row r="316" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C316" s="4"/>
     </row>
-    <row r="317" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C317" s="4"/>
     </row>
-    <row r="318" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C318" s="4"/>
     </row>
-    <row r="319" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C319" s="4"/>
     </row>
-    <row r="320" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C320" s="4"/>
     </row>
-    <row r="321" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C321" s="4"/>
     </row>
-    <row r="322" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C322" s="4"/>
     </row>
-    <row r="323" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C323" s="4"/>
     </row>
-    <row r="324" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C324" s="4"/>
     </row>
-    <row r="325" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C325" s="4"/>
     </row>
-    <row r="326" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C326" s="4"/>
     </row>
-    <row r="327" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C327" s="4"/>
     </row>
-    <row r="328" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C328" s="4"/>
     </row>
-    <row r="329" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C329" s="4"/>
     </row>
-    <row r="330" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C330" s="4"/>
     </row>
-    <row r="331" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C331" s="4"/>
     </row>
-    <row r="332" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C332" s="4"/>
     </row>
-    <row r="333" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C333" s="4"/>
     </row>
-    <row r="334" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C335" s="3"/>
     </row>
-    <row r="336" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C336" s="4"/>
     </row>
-    <row r="337" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C337" s="3"/>
     </row>
-    <row r="338" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C338" s="4"/>
     </row>
-    <row r="339" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C339" s="3"/>
     </row>
-    <row r="340" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C340" s="4"/>
     </row>
-    <row r="341" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C341" s="3"/>
     </row>
-    <row r="342" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C342" s="4"/>
     </row>
-    <row r="343" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C343" s="3"/>
     </row>
-    <row r="344" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C344" s="4"/>
     </row>
-    <row r="345" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C345" s="3"/>
     </row>
-    <row r="346" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C346" s="4"/>
     </row>
-    <row r="347" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C347" s="3"/>
     </row>
-    <row r="348" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C348" s="4"/>
     </row>
-    <row r="349" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C349" s="3"/>
     </row>
-    <row r="350" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C350" s="4"/>
     </row>
-    <row r="351" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C351" s="3"/>
     </row>
-    <row r="352" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C352" s="4"/>
     </row>
-    <row r="353" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C353" s="3"/>
     </row>
-    <row r="354" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C355" s="3"/>
     </row>
-    <row r="356" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C357" s="3"/>
     </row>
-    <row r="358" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C359" s="3"/>
     </row>
-    <row r="360" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C361" s="3"/>
     </row>
-    <row r="362" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C363" s="3"/>
     </row>
-    <row r="364" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C365" s="3"/>
     </row>
-    <row r="366" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C367" s="3"/>
     </row>
-    <row r="368" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C369" s="3"/>
     </row>
-    <row r="370" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C371" s="3"/>
     </row>
-    <row r="372" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C373" s="3"/>
     </row>
-    <row r="374" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C375" s="3"/>
     </row>
-    <row r="376" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C377" s="3"/>
     </row>
-    <row r="378" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C379" s="3"/>
     </row>
-    <row r="380" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C381" s="3"/>
     </row>
-    <row r="382" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C383" s="3"/>
     </row>
-    <row r="384" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C385" s="3"/>
     </row>
-    <row r="386" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C387" s="3"/>
     </row>
-    <row r="388" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C388" s="4"/>
     </row>
-    <row r="389" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C389" s="3"/>
     </row>
-    <row r="390" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C390" s="4"/>
     </row>
-    <row r="391" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C391" s="3"/>
     </row>
-    <row r="392" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C392" s="3"/>
     </row>
-    <row r="393" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C393" s="3"/>
     </row>
-    <row r="394" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C394" s="3"/>
     </row>
-    <row r="395" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C395" s="4"/>
     </row>
-    <row r="396" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C396" s="3"/>
     </row>
-    <row r="397" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C397" s="4"/>
     </row>
-    <row r="398" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C398" s="3"/>
     </row>
-    <row r="399" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C399" s="4"/>
     </row>
-    <row r="400" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C400" s="3"/>
     </row>
-    <row r="401" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C402" s="3"/>
     </row>
-    <row r="403" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C403" s="4"/>
     </row>
-    <row r="404" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C404" s="3"/>
     </row>
-    <row r="405" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C405" s="4"/>
     </row>
-    <row r="406" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C406" s="3"/>
     </row>
-    <row r="407" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C407" s="4"/>
     </row>
-    <row r="408" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C408" s="3"/>
     </row>
-    <row r="409" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C410" s="3"/>
     </row>
-    <row r="411" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C411" s="4"/>
     </row>
-    <row r="412" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C412" s="3"/>
     </row>
-    <row r="413" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C413" s="4"/>
     </row>
-    <row r="414" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C414" s="3"/>
     </row>
-    <row r="415" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C415" s="4"/>
     </row>
-    <row r="416" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C416" s="3"/>
     </row>
-    <row r="417" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C417" s="4"/>
     </row>
-    <row r="418" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C418" s="3"/>
     </row>
-    <row r="419" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C419" s="4"/>
     </row>
-    <row r="420" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C420" s="3"/>
     </row>
-    <row r="421" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C421" s="4"/>
     </row>
-    <row r="422" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C422" s="3"/>
     </row>
-    <row r="423" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C423" s="4"/>
     </row>
-    <row r="424" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C424" s="3"/>
     </row>
-    <row r="425" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C425" s="4"/>
     </row>
-    <row r="426" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C426" s="3"/>
     </row>
-    <row r="427" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C427" s="4"/>
     </row>
-    <row r="428" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C428" s="3"/>
     </row>
-    <row r="429" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C429" s="4"/>
     </row>
-    <row r="430" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C430" s="3"/>
     </row>
-    <row r="431" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C431" s="4"/>
     </row>
-    <row r="432" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C432" s="3"/>
     </row>
-    <row r="433" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C433" s="4"/>
     </row>
-    <row r="434" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C434" s="3"/>
     </row>
-    <row r="435" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C435" s="4"/>
     </row>
-    <row r="436" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C436" s="3"/>
     </row>
-    <row r="437" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C438" s="3"/>
     </row>
-    <row r="439" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C439" s="4"/>
     </row>
-    <row r="440" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C440" s="3"/>
     </row>
-    <row r="441" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C441" s="4"/>
     </row>
-    <row r="442" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C442" s="3"/>
     </row>
-    <row r="443" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C443" s="4"/>
     </row>
-    <row r="444" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="444" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C444" s="3"/>
     </row>
-    <row r="445" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C445" s="4"/>
     </row>
-    <row r="446" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C446" s="3"/>
     </row>
-    <row r="447" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C447" s="4"/>
     </row>
-    <row r="448" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C448" s="3"/>
     </row>
-    <row r="449" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C449" s="4"/>
     </row>
-    <row r="450" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C450" s="3"/>
     </row>
-    <row r="451" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C451" s="4"/>
     </row>
-    <row r="452" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C452" s="3"/>
     </row>
-    <row r="453" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="453" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C453" s="4"/>
     </row>
-    <row r="454" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C454" s="3"/>
     </row>
-    <row r="455" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C455" s="3"/>
     </row>
-    <row r="456" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C456" s="3"/>
     </row>
-    <row r="457" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C457" s="4"/>
     </row>
-    <row r="458" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C458" s="3"/>
     </row>
-    <row r="459" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C459" s="4"/>
     </row>
   </sheetData>
@@ -3248,6 +3278,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316A6B2706F22F479EB96B4E836A2AA9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb14f50e3c0e0698014ac1b2b11cfd92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="952decf2-c70e-41dd-b7af-a901e5274ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e289b93c4a0db376190258ac9ef1386" ns3:_="">
     <xsd:import namespace="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
@@ -3403,7 +3441,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3412,15 +3450,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91CA701E-F7B0-428B-9668-E44388524238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3438,20 +3478,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added instructions and some examples
</commit_message>
<xml_diff>
--- a/Templates/Heat_and_Steam.xlsx
+++ b/Templates/Heat_and_Steam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\LevelUPESG\Batch-input-Page\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D9DAA-4FCE-4082-A0B0-87CCCBEF092A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9CBB01-F101-427B-AED1-370411B201BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="196">
   <si>
     <t>Asset Name</t>
   </si>
@@ -508,13 +508,130 @@
   </si>
   <si>
     <t>ZWD</t>
+  </si>
+  <si>
+    <t>The fiscal year for which the data is being reported, e.g., 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of value being recorded, such as Consumption or Total Spend </t>
+  </si>
+  <si>
+    <t>The total amount of energy consumed by the asset during the reporting period, measured in kilowatt-hours (kWh)</t>
+  </si>
+  <si>
+    <t>The specific type of fuel or energy source used</t>
+  </si>
+  <si>
+    <t>The total cost associated with the asset for the reporting period</t>
+  </si>
+  <si>
+    <t>The currency in which the total spend is reported</t>
+  </si>
+  <si>
+    <t>Indicates whether the reported data is an actual measurement or an estimate.</t>
+  </si>
+  <si>
+    <t>If 'Source' is marked as 'Estimated,' please provide a brief explanation in the 'Assumption Basis' column. If the source is actual, write 'N/A'</t>
+  </si>
+  <si>
+    <t>Provide a reference to supporting documentation that verifies the reported data. This could be a link to the invoice or other relevant documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumption </t>
+  </si>
+  <si>
+    <t>link to invoice</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>company1</t>
+  </si>
+  <si>
+    <t>company2</t>
+  </si>
+  <si>
+    <t>company3</t>
+  </si>
+  <si>
+    <t>company4</t>
+  </si>
+  <si>
+    <t>company5</t>
+  </si>
+  <si>
+    <t>company6</t>
+  </si>
+  <si>
+    <t>company7</t>
+  </si>
+  <si>
+    <t>company8</t>
+  </si>
+  <si>
+    <t>company9</t>
+  </si>
+  <si>
+    <t>company10</t>
+  </si>
+  <si>
+    <t>company11</t>
+  </si>
+  <si>
+    <t>estimated</t>
+  </si>
+  <si>
+    <t>reason 1</t>
+  </si>
+  <si>
+    <t>link l</t>
+  </si>
+  <si>
+    <t>reason 2</t>
+  </si>
+  <si>
+    <t>link 2</t>
+  </si>
+  <si>
+    <t>reason 3</t>
+  </si>
+  <si>
+    <t>reason 4</t>
+  </si>
+  <si>
+    <t>link 3</t>
+  </si>
+  <si>
+    <t>reason 5</t>
+  </si>
+  <si>
+    <t>reason 6</t>
+  </si>
+  <si>
+    <t>link 4</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>link 5</t>
+  </si>
+  <si>
+    <t>link 6</t>
+  </si>
+  <si>
+    <t>link 7</t>
+  </si>
+  <si>
+    <t>District heat and steam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +668,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1128,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D775E0E9-E192-457C-A3B8-47F95293021D}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1185,81 +1308,434 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="1">
+        <v>300</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="I7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1">
+        <v>400</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
+      <c r="J10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>600</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12">
+        <v>2023</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:F1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$D2 &lt;&gt; "Consumption "</formula>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="E4:F1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$D4 &lt;&gt; "Consumption "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H1048575">
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$D2 &lt;&gt; "Total Spend"</formula>
+  <conditionalFormatting sqref="G3:H1048575">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D3 &lt;&gt; "Total Spend"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{F8764847-9C39-4CD8-A2DB-642B0361E72F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I1048576" xr:uid="{F8764847-9C39-4CD8-A2DB-642B0361E72F}">
       <formula1>"estimated, actual"</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{F95358CC-E00E-45D8-9D22-D49F2BC6ABF5}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{E8E9EA8B-F502-456B-8568-B3A4675F91E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576" xr:uid="{E8E9EA8B-F502-456B-8568-B3A4675F91E0}">
       <formula1>"Consumption ,Total Spend"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 C1:C2" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1 D4:D1048576" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
       <formula1>2020</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{06635ADA-7664-4747-91AB-2EB240994011}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{06635ADA-7664-4747-91AB-2EB240994011}">
       <formula1>"Onsite heat and steam,District heat and steam"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3:B1048576" xr:uid="{C8B4DF01-70D4-4C4C-B6B9-547A38C4AF08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B1048576" xr:uid="{C8B4DF01-70D4-4C4C-B6B9-547A38C4AF08}">
       <formula1>"Heat and Steam"</formula1>
     </dataValidation>
-    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{9DEC22D6-A9B9-4942-B6B3-A759EF71BB17}">
-      <formula1>$D2 = "Consumption "</formula1>
+    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E1048576" xr:uid="{9DEC22D6-A9B9-4942-B6B3-A759EF71BB17}">
+      <formula1>$D4 = "Consumption "</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{A931B69C-F657-4E55-A7D7-D60577855578}">
-      <formula1>$D2 = "Total Spend"</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1048576" xr:uid="{A931B69C-F657-4E55-A7D7-D60577855578}">
+      <formula1>$D4 = "Total Spend"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{45605CBE-FD23-4A0E-A03A-B5C065317735}">
       <formula1>2020</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1268,7 +1744,7 @@
           <x14:formula1>
             <xm:f>data!$A$2:$A$182</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>H4:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3218,6 +3694,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316A6B2706F22F479EB96B4E836A2AA9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb14f50e3c0e0698014ac1b2b11cfd92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="952decf2-c70e-41dd-b7af-a901e5274ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e289b93c4a0db376190258ac9ef1386" ns3:_="">
     <xsd:import namespace="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
@@ -3373,24 +3866,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91CA701E-F7B0-428B-9668-E44388524238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3406,22 +3900,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tested heat and steam
</commit_message>
<xml_diff>
--- a/Templates/Heat_and_Steam.xlsx
+++ b/Templates/Heat_and_Steam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemoa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\LevelUPESG\Batch-input-Page\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7449AC62-03CD-45C3-8329-381659D9D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F588D0-C327-4BC8-B27A-9353A1C0EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="14100" windowHeight="11076" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat and Steam" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="176">
   <si>
     <t>Asset Name</t>
   </si>
@@ -513,9 +513,6 @@
     <t xml:space="preserve">Consumption </t>
   </si>
   <si>
-    <t>District heat and steam</t>
-  </si>
-  <si>
     <t>The fiscal year for which the data is being reported, e.g., 2021</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>company2</t>
   </si>
   <si>
-    <t>company3</t>
-  </si>
-  <si>
     <t>reason 2</t>
   </si>
   <si>
@@ -571,9 +565,6 @@
   </si>
   <si>
     <t>link 2</t>
-  </si>
-  <si>
-    <t>link 3</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D775E0E9-E192-457C-A3B8-47F95293021D}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,36 +1276,36 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -1335,15 +1326,15 @@
         <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -1352,27 +1343,33 @@
         <v>2023</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>2000</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>158</v>
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <v>30</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>156</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -1381,7 +1378,10 @@
         <v>2023</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>157</v>
+      </c>
+      <c r="E5" s="1">
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>13</v>
@@ -1396,42 +1396,10 @@
         <v>156</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2023</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="1">
-        <v>500</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1441,12 +1409,12 @@
       <formula>$D3 &lt;&gt; "Consumption "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:F1 E3:F1048576">
+  <conditionalFormatting sqref="E3:F1048576 E1:F1">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D:$D="Total Spend"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1 G3:H1048576">
+  <conditionalFormatting sqref="G3:H1048576 G1:H1">
     <cfRule type="expression" dxfId="1" priority="5">
       <formula>$D:$D ="Consumption"</formula>
     </cfRule>
@@ -3443,6 +3411,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316A6B2706F22F479EB96B4E836A2AA9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb14f50e3c0e0698014ac1b2b11cfd92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="952decf2-c70e-41dd-b7af-a901e5274ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e289b93c4a0db376190258ac9ef1386" ns3:_="">
     <xsd:import namespace="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
@@ -3598,24 +3583,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91CA701E-F7B0-428B-9668-E44388524238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3631,22 +3617,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>